<commit_message>
added til og med P=29
</commit_message>
<xml_diff>
--- a/data/data_staffing_constraint.xlsx
+++ b/data/data_staffing_constraint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiebach/Documents/11. semester/Speciale/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiebach/Documents/11. semester/git/Speciale/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF56848-7EAB-654B-99FE-71BC93C64A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B0D451-9764-6B48-8A3F-5249EBDE9614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="3" xr2:uid="{D565E627-EA86-6D43-8C3B-D6B81E8A39CD}"/>
+    <workbookView xWindow="28800" yWindow="-1840" windowWidth="16500" windowHeight="19700" activeTab="3" xr2:uid="{D565E627-EA86-6D43-8C3B-D6B81E8A39CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="40">
   <si>
     <t>DR1</t>
   </si>
@@ -115,12 +115,6 @@
     <t>DR Radio</t>
   </si>
   <si>
-    <t>Podcast</t>
-  </si>
-  <si>
-    <t>Mixtape</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>Scope</t>
+  </si>
+  <si>
+    <t>Dilemma - Stacking</t>
+  </si>
+  <si>
+    <t>Dilemma - Binge</t>
   </si>
 </sst>
 </file>
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE725C8-397A-7649-831D-85A70EAC0DA1}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C40"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,19 +530,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
       <c r="I1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -559,7 +559,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -593,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -882,10 +882,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -893,7 +893,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -904,7 +904,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -915,7 +915,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -926,7 +926,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -937,7 +937,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -948,7 +948,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -959,10 +959,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -970,32 +970,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1006,40 +984,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CCA602-F503-6F49-9FFF-98C828BDF155}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1418,7 +1396,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>21</v>
@@ -1691,22 +1669,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1714,7 +1692,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -1737,7 +1715,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -1760,7 +1738,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -1783,7 +1761,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -1806,7 +1784,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -1829,7 +1807,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -1852,22 +1830,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F37">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1875,68 +1853,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F38">
         <v>7</v>
       </c>
       <c r="G38">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>4</v>
-      </c>
-      <c r="F39">
-        <v>7</v>
-      </c>
-      <c r="G39">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40">
-        <v>7</v>
-      </c>
-      <c r="G40">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1956,21 +1888,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -1990,7 +1922,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2010,7 +1942,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>2.4</v>
@@ -2030,7 +1962,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -2055,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32586BF-3937-3043-9D34-356F3B403458}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2069,16 +2001,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2313,10 +2245,10 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
         <v>6</v>
-      </c>
-      <c r="D18">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2478,13 +2410,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D30">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2492,7 +2424,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -2506,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
@@ -2520,13 +2452,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
       </c>
       <c r="D33">
-        <v>104</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2534,13 +2466,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
       <c r="D34">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2548,7 +2480,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -2562,7 +2494,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -2576,13 +2508,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2590,41 +2522,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" t="s">
         <v>6</v>
-      </c>
-      <c r="D39">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added type and names in data
</commit_message>
<xml_diff>
--- a/data/data_staffing_constraint.xlsx
+++ b/data/data_staffing_constraint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3669516081e98610/Dokumenter/Uni/Speciale/Git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D6F34D45-E6EF-8641-99C3-E02BD3517319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB7991AB-F631-427F-9607-5DE6958658AC}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{D6F34D45-E6EF-8641-99C3-E02BD3517319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B76BC6B7-B236-4B45-9EBF-03B0B6DD5B7D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{D565E627-EA86-6D43-8C3B-D6B81E8A39CD}"/>
+    <workbookView xWindow="28702" yWindow="-2543" windowWidth="21795" windowHeight="12975" xr2:uid="{D565E627-EA86-6D43-8C3B-D6B81E8A39CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="47">
   <si>
     <t>DR1</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>DIGITAL</t>
+  </si>
+  <si>
+    <t>TYPE</t>
   </si>
 </sst>
 </file>
@@ -235,6 +238,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,17 +543,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE725C8-397A-7649-831D-85A70EAC0DA1}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -556,6 +563,9 @@
       <c r="C1" t="s">
         <v>27</v>
       </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
       <c r="I1" t="s">
         <v>25</v>
       </c>
@@ -563,7 +573,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -573,6 +583,9 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
       <c r="I2">
         <v>1</v>
       </c>
@@ -580,7 +593,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -590,6 +603,9 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
       <c r="I3">
         <v>2</v>
       </c>
@@ -597,7 +613,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -607,6 +623,9 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
       <c r="I4">
         <v>3</v>
       </c>
@@ -614,7 +633,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,6 +643,9 @@
       <c r="C5" t="s">
         <v>39</v>
       </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
       <c r="I5">
         <v>4</v>
       </c>
@@ -631,7 +653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -641,8 +663,11 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -652,8 +677,11 @@
       <c r="C7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -663,8 +691,11 @@
       <c r="C8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -674,8 +705,11 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -685,8 +719,11 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -696,8 +733,11 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -707,8 +747,11 @@
       <c r="C12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -718,8 +761,11 @@
       <c r="C13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -729,8 +775,11 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -740,8 +789,11 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -751,8 +803,11 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -762,8 +817,11 @@
       <c r="C17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -773,8 +831,11 @@
       <c r="C18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -784,8 +845,11 @@
       <c r="C19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -795,8 +859,11 @@
       <c r="C20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -806,8 +873,11 @@
       <c r="C21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -817,8 +887,11 @@
       <c r="C22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -828,8 +901,11 @@
       <c r="C23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -839,8 +915,11 @@
       <c r="C24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -850,8 +929,11 @@
       <c r="C25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -861,8 +943,11 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -872,8 +957,11 @@
       <c r="C27" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -883,8 +971,11 @@
       <c r="C28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -894,8 +985,11 @@
       <c r="C29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -905,8 +999,11 @@
       <c r="C30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -916,8 +1013,11 @@
       <c r="C31" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -927,8 +1027,11 @@
       <c r="C32" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -938,8 +1041,11 @@
       <c r="C33" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -949,8 +1055,11 @@
       <c r="C34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -960,8 +1069,11 @@
       <c r="C35" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -971,8 +1083,11 @@
       <c r="C36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -982,8 +1097,11 @@
       <c r="C37" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -992,6 +1110,9 @@
       </c>
       <c r="C38" t="s">
         <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1008,14 +1129,14 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="22.1875" customWidth="1"/>
+    <col min="3" max="3" width="22.25" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1159,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1061,7 +1182,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1084,7 +1205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1107,7 +1228,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1130,7 +1251,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1153,7 +1274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1176,7 +1297,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1199,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1222,7 +1343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1245,7 +1366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1268,7 +1389,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1291,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1314,7 +1435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1337,7 +1458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1360,7 +1481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1383,7 +1504,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1406,7 +1527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1429,7 +1550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1452,7 +1573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1475,7 +1596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1498,7 +1619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1521,7 +1642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1544,7 +1665,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1567,7 +1688,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1590,7 +1711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1613,7 +1734,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1636,7 +1757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1659,7 +1780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1682,7 +1803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1705,7 +1826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1728,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1751,7 +1872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1774,7 +1895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1797,7 +1918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1820,7 +1941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1843,7 +1964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1866,7 +1987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1902,9 +2023,9 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>33</v>
       </c>
@@ -1918,7 +2039,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1938,7 +2059,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1958,7 +2079,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1978,7 +2099,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2007,17 +2128,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32586BF-3937-3043-9D34-356F3B403458}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -2031,7 +2152,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2045,7 +2166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2059,7 +2180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2073,7 +2194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2087,7 +2208,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2101,7 +2222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2115,7 +2236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2129,7 +2250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2143,7 +2264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2157,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2171,7 +2292,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2185,7 +2306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2199,7 +2320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2213,7 +2334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2227,7 +2348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2241,7 +2362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2255,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2269,7 +2390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2283,7 +2404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2297,7 +2418,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2311,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2325,7 +2446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2339,7 +2460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2353,7 +2474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2367,7 +2488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2381,7 +2502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2395,7 +2516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2409,7 +2530,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2423,7 +2544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2437,7 +2558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2451,7 +2572,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2465,7 +2586,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2479,7 +2600,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2493,7 +2614,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2507,7 +2628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2521,7 +2642,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2535,7 +2656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>

</xml_diff>